<commit_message>
Add row sum results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/Single cell/knock_out_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A7ECE3-73AC-7246-99DD-1E26A837EBB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80949444-EC09-8446-B2EE-016FA45F8FDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{F4360573-7EBD-014D-BAFF-FA13112AF2FE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="3" xr2:uid="{F4360573-7EBD-014D-BAFF-FA13112AF2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="NKX2-1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="29">
   <si>
     <t>method</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>211(=0.1)</t>
+  </si>
+  <si>
+    <t>Trivial col</t>
+  </si>
+  <si>
+    <t>Trivial column</t>
+  </si>
+  <si>
+    <t>row_sum_row</t>
+  </si>
+  <si>
+    <t>row_sum_col</t>
+  </si>
+  <si>
+    <t>row_sum_both</t>
   </si>
 </sst>
 </file>
@@ -185,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -220,6 +235,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A72741-1863-E34F-B28D-C9F653EDFE3E}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,10 +566,9 @@
     <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.5" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -917,7 +934,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -937,14 +954,26 @@
         <v>18</v>
       </c>
       <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>171</v>
       </c>
       <c r="C21" s="2"/>
@@ -953,7 +982,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -968,7 +997,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1014,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -998,13 +1027,13 @@
       <c r="D24" s="2">
         <v>174</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="5">
         <v>189</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1025,7 +1054,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1048,78 +1077,161 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
         <v>76</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="11">
         <v>101</v>
       </c>
       <c r="D27" s="2">
         <v>28</v>
       </c>
-      <c r="E27" s="4">
+      <c r="H27" s="14">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>109</v>
+      </c>
+      <c r="C28" s="2">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>174</v>
+      </c>
+      <c r="H28">
         <v>36</v>
       </c>
-      <c r="F27" s="2">
+      <c r="I28" s="15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>94</v>
+      </c>
+      <c r="C29" s="2">
+        <v>27</v>
+      </c>
+      <c r="D29" s="12">
+        <v>207</v>
+      </c>
+      <c r="H29">
+        <v>28</v>
+      </c>
+      <c r="I29">
+        <v>174</v>
+      </c>
+      <c r="J29" s="16">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2">
+        <v>76</v>
+      </c>
+      <c r="C30" s="2">
         <v>101</v>
       </c>
-      <c r="G27" s="2">
+      <c r="D30" s="2">
         <v>28</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="E30" s="4">
+        <v>36</v>
+      </c>
+      <c r="F30" s="2">
+        <v>101</v>
+      </c>
+      <c r="G30" s="2">
+        <v>28</v>
+      </c>
+      <c r="H30" s="2">
+        <v>104</v>
+      </c>
+      <c r="I30" s="2">
+        <v>36</v>
+      </c>
+      <c r="J30" s="2">
+        <v>28</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>74</v>
+      </c>
+      <c r="E31" s="2">
+        <v>35</v>
+      </c>
+      <c r="L31">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="B33" s="2">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2">
         <v>4</v>
       </c>
-      <c r="E29" s="4">
-        <v>5</v>
-      </c>
-      <c r="F29" s="4">
-        <v>5</v>
-      </c>
-      <c r="G29" s="4">
+      <c r="E33" s="4">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4">
+        <v>5</v>
+      </c>
+      <c r="G33" s="4">
         <v>4</v>
       </c>
-      <c r="H29" s="2">
+      <c r="K33" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1131,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB954FE8-A101-7B40-9A27-7BCA09296252}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1472,7 +1584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -1492,14 +1604,26 @@
         <v>18</v>
       </c>
       <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>128</v>
       </c>
       <c r="C21" s="2"/>
@@ -1508,7 +1632,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1523,7 +1647,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1540,7 +1664,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1553,13 +1677,13 @@
       <c r="D24" s="2">
         <v>50</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="5">
         <v>79</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1580,7 +1704,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1603,78 +1727,164 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
         <v>72</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="11">
         <v>114</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2">
+        <v>14</v>
+      </c>
+      <c r="H27" s="11">
+        <v>116</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>83</v>
+      </c>
+      <c r="C28" s="2">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>49</v>
+      </c>
+      <c r="H28" s="2">
+        <v>35</v>
+      </c>
+      <c r="I28" s="5">
+        <v>85</v>
+      </c>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>51</v>
+      </c>
+      <c r="C29" s="2">
+        <v>14</v>
+      </c>
+      <c r="D29" s="12">
+        <v>79</v>
+      </c>
+      <c r="H29" s="2">
+        <v>14</v>
+      </c>
+      <c r="I29" s="2">
+        <v>52</v>
+      </c>
+      <c r="J29" s="12">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2">
+        <v>114</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E30" s="2">
         <v>31</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F30" s="2">
         <v>114</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H30" s="2">
+        <v>116</v>
+      </c>
+      <c r="I30" s="2">
+        <v>35</v>
+      </c>
+      <c r="J30" s="2">
+        <v>14</v>
+      </c>
+      <c r="K30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2">
+        <v>71</v>
+      </c>
+      <c r="E31" s="2">
+        <v>31</v>
+      </c>
+      <c r="L31">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B33" s="2">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
         <v>4</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D33" s="2">
         <v>1</v>
       </c>
-      <c r="E29" s="4">
-        <v>5</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="E33" s="4">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4">
         <v>4</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G33" s="4">
         <v>2</v>
       </c>
-      <c r="H29" s="4">
+      <c r="K33" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1689,7 +1899,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2208,10 +2418,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3529FA7D-7F88-804F-8970-1B73A3313F65}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2223,8 +2433,9 @@
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2591,7 +2802,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -2610,15 +2821,24 @@
       <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>65</v>
       </c>
       <c r="C21" s="2"/>
@@ -2627,7 +2847,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2642,7 +2862,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2659,7 +2879,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2672,13 +2892,13 @@
       <c r="D24" s="2">
         <v>54</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="5">
         <v>65</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2699,7 +2919,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2722,75 +2942,153 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="11">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>52</v>
+      </c>
+      <c r="C28" s="2">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2">
+        <v>52</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>54</v>
+      </c>
+      <c r="C29" s="2">
+        <v>27</v>
+      </c>
+      <c r="D29" s="12">
+        <v>55</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>53</v>
+      </c>
+      <c r="J29" s="16">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B30" s="4">
         <v>63</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C30" s="4">
         <v>89</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D30" s="4">
         <v>53</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E30" s="4">
         <v>63</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F30" s="2">
         <v>89</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G30" s="2">
         <v>53</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>54</v>
+      </c>
+      <c r="J30" s="4">
+        <v>53</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B32" s="2">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="4">
-        <v>5</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4">
+        <v>5</v>
+      </c>
+      <c r="F32" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G32" s="4">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>5</v>
+      </c>
+      <c r="J32" s="4">
         <v>5</v>
       </c>
     </row>

</xml_diff>